<commit_message>
DMS: Fix KpiProductGrouping Import
</commit_message>
<xml_diff>
--- a/DMS/Templates/Kpi_Product_Grouping_Export.xlsx
+++ b/DMS/Templates/Kpi_Product_Grouping_Export.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dotNet\DMS\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793A1460-CDDE-4EE3-BD1E-572707638FD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580264E6-35D3-4B74-A55F-71E262930065}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,28 +108,28 @@
     <t>{{KpiProductGroupings.Employees.DisplayName}}</t>
   </si>
   <si>
-    <t>{{KpiProductGroupings.Employees.KpiProductGroupingTypeName}}</t>
-  </si>
-  <si>
-    <t>{{KpiProductGroupings.Employees.ProductGroupings.Code}}</t>
-  </si>
-  <si>
-    <t>{{KpiProductGroupings.Employees.ProductGroupings.Name}}</t>
-  </si>
-  <si>
-    <t>{{KpiProductGroupings.Employees.ProductGroupings.ItemCount}}</t>
-  </si>
-  <si>
-    <t>{{KpiProductGroupings.Employees.ProductGroupings.Items.Code}}</t>
-  </si>
-  <si>
-    <t>{{KpiProductGroupings.Employees.ProductGroupings.Items.Name}}</t>
-  </si>
-  <si>
-    <t>{{KpiProductGroupings.Employees.ProductGroupings.Items.IndirectRevenue}}</t>
-  </si>
-  <si>
-    <t>{{KpiProductGroupings.Employees.ProductGroupings.Items.IndirectStoreCounter}}</t>
+    <t>{{KpiProductGroupings.Employees.KpiProductGroupings.KpiProductGroupingTypeName}}</t>
+  </si>
+  <si>
+    <t>{{KpiProductGroupings.Employees.KpiProductGroupings.Contents.Code}}</t>
+  </si>
+  <si>
+    <t>{{KpiProductGroupings.Employees.KpiProductGroupings.Contents.Name}}</t>
+  </si>
+  <si>
+    <t>{{KpiProductGroupings.Employees.KpiProductGroupings.Contents.ItemCount}}</t>
+  </si>
+  <si>
+    <t>{{KpiProductGroupings.Employees.KpiProductGroupings.Contents.Items.Code}}</t>
+  </si>
+  <si>
+    <t>{{KpiProductGroupings.Employees.KpiProductGroupings.Contents.Items.Name}}</t>
+  </si>
+  <si>
+    <t>{{KpiProductGroupings.Employees.KpiProductGroupings.Contents.Items.IndirectRevenue}}</t>
+  </si>
+  <si>
+    <t>{{KpiProductGroupings.Employees.KpiProductGroupings.Contents.Items.IndirectStoreCounter}}</t>
   </si>
 </sst>
 </file>
@@ -274,6 +274,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -282,9 +285,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -572,7 +572,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -583,40 +583,41 @@
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="29.85546875" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="8" width="31.28515625" customWidth="1"/>
+    <col min="7" max="7" width="73.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="74.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30.28515625" customWidth="1"/>
     <col min="10" max="10" width="22.42578125" customWidth="1"/>
     <col min="11" max="11" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -651,37 +652,37 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="9" t="s">
@@ -698,33 +699,33 @@
       </c>
     </row>
     <row r="7" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="11"/>

</xml_diff>

<commit_message>
DMS: Update KpiProductGrouping Export template
</commit_message>
<xml_diff>
--- a/DMS/Templates/Kpi_Product_Grouping_Export.xlsx
+++ b/DMS/Templates/Kpi_Product_Grouping_Export.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dotNet\DMS\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580264E6-35D3-4B74-A55F-71E262930065}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB946064-3C68-4703-8E68-3DE3AB522036}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPI nhóm sản phẩm" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'KPI nhóm sản phẩm'!$A$4:$D$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'KPI nhóm sản phẩm'!$A$4:$G$4</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -196,7 +196,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -241,11 +241,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -256,12 +269,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -285,6 +292,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -569,179 +591,244 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="62.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="73.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="74.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" customWidth="1"/>
-    <col min="11" max="11" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" customWidth="1"/>
+    <col min="11" max="12" width="11.42578125" customWidth="1"/>
+    <col min="13" max="13" width="24.42578125" customWidth="1"/>
+    <col min="14" max="14" width="32.140625" customWidth="1"/>
+    <col min="15" max="15" width="30.28515625" customWidth="1"/>
+    <col min="16" max="16" width="22.42578125" customWidth="1"/>
+    <col min="17" max="17" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="2"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="16"/>
+      <c r="E4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="16"/>
+      <c r="G4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="H4" s="16"/>
+      <c r="I4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="J4" s="16"/>
+      <c r="K4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="L4" s="16"/>
+      <c r="M4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="8"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="6"/>
     </row>
-    <row r="6" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="F6" s="14"/>
+      <c r="G6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="H6" s="14"/>
+      <c r="I6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="J6" s="14"/>
+      <c r="K6" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="L6" s="14"/>
+      <c r="M6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="N6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="O6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="P6" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
+    <row r="7" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
+    <row r="8" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
+    <row r="9" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A5:J5"/>
+  <mergeCells count="15">
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A2:P2"/>
+    <mergeCell ref="A5:P5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K6:L6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
DMS: Fix Kpi ProductGrouping Import
</commit_message>
<xml_diff>
--- a/DMS/Templates/Kpi_Product_Grouping_Export.xlsx
+++ b/DMS/Templates/Kpi_Product_Grouping_Export.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dotNet\DMS\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB946064-3C68-4703-8E68-3DE3AB522036}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C191247D-35DE-43C2-A9CD-0EBDAD405BD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="KPI nhóm sản phẩm" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'KPI nhóm sản phẩm'!$A$4:$G$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'KPI nhóm sản phẩm'!$A$4:$L$4</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -63,42 +63,6 @@
     <t>Số sản phẩm</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Kỳ: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">{{KpiPeriod}} - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Năm: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{{KpiYear}}</t>
-    </r>
-  </si>
-  <si>
     <t>{{KpiProductGroupings.OrganizationName}}</t>
   </si>
   <si>
@@ -126,10 +90,13 @@
     <t>{{KpiProductGroupings.Employees.KpiProductGroupings.Contents.Items.Name}}</t>
   </si>
   <si>
-    <t>{{KpiProductGroupings.Employees.KpiProductGroupings.Contents.Items.IndirectRevenue}}</t>
-  </si>
-  <si>
-    <t>{{KpiProductGroupings.Employees.KpiProductGroupings.Contents.Items.IndirectStoreCounter}}</t>
+    <t>{{KpiProductGroupings.Employees.KpiProductGroupings.Contents.IndirectRevenue}}</t>
+  </si>
+  <si>
+    <t>{{KpiProductGroupings.Employees.KpiProductGroupings.Contents.IndirectStoreCounter}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -170,7 +137,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,14 +156,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -220,15 +181,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -246,6 +198,26 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -258,20 +230,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -290,23 +257,50 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -591,244 +585,305 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6:L6"/>
+      <selection activeCell="A5" sqref="A5:W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" customWidth="1"/>
-    <col min="7" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" customWidth="1"/>
-    <col min="11" max="12" width="11.42578125" customWidth="1"/>
-    <col min="13" max="13" width="24.42578125" customWidth="1"/>
-    <col min="14" max="14" width="32.140625" customWidth="1"/>
-    <col min="15" max="15" width="30.28515625" customWidth="1"/>
-    <col min="16" max="16" width="22.42578125" customWidth="1"/>
-    <col min="17" max="17" width="30.28515625" customWidth="1"/>
+    <col min="2" max="4" width="5.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" customWidth="1"/>
+    <col min="10" max="11" width="9.42578125" customWidth="1"/>
+    <col min="12" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" customWidth="1"/>
+    <col min="16" max="17" width="11.42578125" customWidth="1"/>
+    <col min="18" max="18" width="24.42578125" customWidth="1"/>
+    <col min="19" max="19" width="32.140625" customWidth="1"/>
+    <col min="20" max="20" width="10.28515625" customWidth="1"/>
+    <col min="21" max="21" width="9.28515625" customWidth="1"/>
+    <col min="22" max="22" width="8.42578125" customWidth="1"/>
+    <col min="23" max="23" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="2"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="8"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="9"/>
+    </row>
+    <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="18"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="11"/>
+      <c r="N4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" s="11"/>
+      <c r="P4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="U4" s="14"/>
+      <c r="V4" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="W4" s="21"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="24"/>
+      <c r="V5" s="24"/>
+      <c r="W5" s="24"/>
     </row>
-    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="16"/>
-      <c r="I4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" s="16"/>
-      <c r="K4" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="16"/>
-      <c r="M4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>3</v>
-      </c>
+    <row r="6" spans="1:23" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T6" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="W6" s="19"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="6"/>
-    </row>
-    <row r="6" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" s="14"/>
-      <c r="M6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
+    <row r="7" spans="1:23" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
     </row>
-    <row r="8" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
+    <row r="8" spans="1:23" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
     </row>
-    <row r="9" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
+    <row r="9" spans="1:23" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
       <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="A5:P5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K6:L6"/>
+  <mergeCells count="19">
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="A1:V1"/>
+    <mergeCell ref="A2:V2"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="A5:W5"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="T6:U6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>